<commit_message>
new version and ttl.-file
</commit_message>
<xml_diff>
--- a/ontology/ontology_tables/product_pass_ontology.xlsx
+++ b/ontology/ontology_tables/product_pass_ontology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\product-knowledge\ontology\ontology_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D73DF8-302C-48D1-A8E9-B281E4EB4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324231B2-D749-4711-A0CF-3E7D525CD319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12915" yWindow="15" windowWidth="12795" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="163">
   <si>
     <t>type</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>Identifikation</t>
+  </si>
+  <si>
+    <t>xsd:dateTime</t>
   </si>
 </sst>
 </file>
@@ -601,23 +604,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <font>
-        <color rgb="FF800080"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
+  <dxfs count="54">
     <dxf>
       <font>
         <color rgb="FF800080"/>
@@ -1240,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1413,7 +1400,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>155</v>
@@ -1427,7 +1414,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>155</v>
@@ -1455,7 +1442,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>155</v>
@@ -1732,7 +1719,7 @@
         <v>155</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>151</v>
@@ -1752,7 +1739,7 @@
         <v>155</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>96</v>
@@ -2630,74 +2617,93 @@
         <v>122</v>
       </c>
     </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A66:A70 A72:A79 A81:A1026 A1:A9 A26:A35 A44:A51 A13:A22">
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+  <conditionalFormatting sqref="A66:A70 A72:A79 A81:A84 A1:A9 A26:A35 A44:A51 A13:A22 A86:A1026">
+    <cfRule type="cellIs" dxfId="53" priority="67" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="68" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="69" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:A37 A39">
-    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="65" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="66" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40 A42">
-    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="61" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="62" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="63" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="57" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="cellIs" dxfId="41" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="50" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+      <formula>"relation"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+      <formula>"attribute"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57 A61:A64">
     <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2708,7 +2714,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57 A61:A64">
+  <conditionalFormatting sqref="A65">
     <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2719,7 +2725,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
+  <conditionalFormatting sqref="A71">
     <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2730,7 +2736,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
+  <conditionalFormatting sqref="A58:A60">
     <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2741,18 +2747,18 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58:A60">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+  <conditionalFormatting sqref="A55:A56">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"class"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:A56">
+  <conditionalFormatting sqref="A53:A54">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2763,7 +2769,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:A54">
+  <conditionalFormatting sqref="A80">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2774,7 +2780,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
+  <conditionalFormatting sqref="A23:A25">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2785,7 +2791,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A25">
+  <conditionalFormatting sqref="A10">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2796,7 +2802,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A11:A12">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
@@ -2807,7 +2813,7 @@
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A12">
+  <conditionalFormatting sqref="A85">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>

</xml_diff>